<commit_message>
Projeto Simulacoes de Credito
</commit_message>
<xml_diff>
--- a/src/main/resources/massa.xlsx
+++ b/src/main/resources/massa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cless\workspace-eclipse\projeto-qa-automacao\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7545A9D4-AB4D-4BD5-88FD-8E3D3F35FA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75927A9A-205A-425C-978A-12B4B03A72CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="450" windowWidth="18030" windowHeight="9825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjetoUm" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>customer_name</t>
   </si>
@@ -108,6 +108,39 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>cpf_api</t>
+  </si>
+  <si>
+    <t>97093236014</t>
+  </si>
+  <si>
+    <t>60094146012</t>
+  </si>
+  <si>
+    <t>84809766080</t>
+  </si>
+  <si>
+    <t>62648716050</t>
+  </si>
+  <si>
+    <t>26276298085</t>
+  </si>
+  <si>
+    <t>01317496094</t>
+  </si>
+  <si>
+    <t>55856777050</t>
+  </si>
+  <si>
+    <t>19626829001</t>
+  </si>
+  <si>
+    <t>24094592008</t>
+  </si>
+  <si>
+    <t>58063164083</t>
   </si>
 </sst>
 </file>
@@ -499,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,9 +551,10 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,8 +591,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -595,21 +632,60 @@
       <c r="L2" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>